<commit_message>
arquivo xlxs e merge
</commit_message>
<xml_diff>
--- a/clubes.xlsx
+++ b/clubes.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03092181794\Desktop\R\cartola\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="clubes" sheetId="1" r:id="rId4"/>
+    <sheet name="clubes" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
   <si>
     <t>rank</t>
   </si>
@@ -107,83 +115,128 @@
   </si>
   <si>
     <t>Ceará</t>
+  </si>
+  <si>
+    <t>UF</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>RJ</t>
+  </si>
+  <si>
+    <t>MG</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>GO</t>
+  </si>
+  <si>
+    <t>CE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -373,25 +426,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="16.29"/>
-    <col customWidth="1" min="4" max="4" width="20.14"/>
-    <col customWidth="1" min="5" max="5" width="18.57"/>
+    <col min="3" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -402,17 +460,20 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2">
+      <c r="G1" s="2"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>5</v>
@@ -420,16 +481,19 @@
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="5">
         <v>688.6</v>
       </c>
-      <c r="E2" s="5">
+      <c r="F2" s="5">
         <v>30.7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -437,16 +501,19 @@
       <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5">
-        <v>543.0</v>
+      <c r="D3" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="E3" s="5">
+        <v>543</v>
+      </c>
+      <c r="F3" s="5">
         <v>45.8</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>9</v>
@@ -454,16 +521,19 @@
       <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="5">
         <v>466.9</v>
       </c>
-      <c r="E4" s="5">
+      <c r="F4" s="5">
         <v>-18.7</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>6</v>
@@ -471,16 +541,19 @@
       <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="5">
         <v>424.5</v>
       </c>
-      <c r="E5" s="5">
+      <c r="F5" s="5">
         <v>7.2</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>10</v>
@@ -488,16 +561,19 @@
       <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="5">
-        <v>402.0</v>
+      <c r="D6" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="E6" s="5">
-        <v>54.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>402</v>
+      </c>
+      <c r="F6" s="5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>12</v>
@@ -505,16 +581,19 @@
       <c r="C7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="5">
         <v>386.8</v>
       </c>
-      <c r="E7" s="5">
+      <c r="F7" s="5">
         <v>-27.2</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>14</v>
@@ -522,16 +601,19 @@
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="5">
         <v>297.3</v>
       </c>
-      <c r="E8" s="5">
+      <c r="F8" s="5">
         <v>-1.4</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>15</v>
@@ -539,16 +621,19 @@
       <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="5">
         <v>293.2</v>
       </c>
-      <c r="E9" s="5">
+      <c r="F9" s="5">
         <v>-9.5</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>16</v>
@@ -556,16 +641,19 @@
       <c r="C10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="5">
-        <v>260.9</v>
+      <c r="D10" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="E10" s="5">
-        <v>64.9</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>260.89999999999998</v>
+      </c>
+      <c r="F10" s="5">
+        <v>64.900000000000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>17</v>
@@ -573,16 +661,19 @@
       <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="5">
-        <v>257.9</v>
+      <c r="D11" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="E11" s="5">
+        <v>257.89999999999998</v>
+      </c>
+      <c r="F11" s="5">
         <v>-21.8</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>18</v>
@@ -590,16 +681,19 @@
       <c r="C12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="5">
         <v>217.7</v>
       </c>
-      <c r="E12" s="5">
+      <c r="F12" s="5">
         <v>-77.3</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>19</v>
@@ -607,16 +701,19 @@
       <c r="C13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="5">
         <v>207.4</v>
       </c>
-      <c r="E13" s="5">
-        <v>16.4</v>
-      </c>
-    </row>
-    <row r="14">
+      <c r="F13" s="5">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>21</v>
@@ -624,16 +721,19 @@
       <c r="C14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="5">
         <v>182.9</v>
       </c>
-      <c r="E14" s="5">
+      <c r="F14" s="5">
         <v>-17.2</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>22</v>
@@ -641,16 +741,19 @@
       <c r="C15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="5">
         <v>136.1</v>
       </c>
-      <c r="E15" s="5">
-        <v>4.4</v>
-      </c>
-    </row>
-    <row r="16">
+      <c r="F15" s="5">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>23</v>
@@ -658,16 +761,19 @@
       <c r="C16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="5">
         <v>104.1</v>
       </c>
-      <c r="E16" s="5">
+      <c r="F16" s="5">
         <v>-14.3</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>25</v>
@@ -675,16 +781,19 @@
       <c r="C17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="5">
         <v>102.8</v>
       </c>
-      <c r="E17" s="5">
+      <c r="F17" s="5">
         <v>2.6</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>26</v>
@@ -692,16 +801,19 @@
       <c r="C18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="5">
         <v>88.3</v>
       </c>
-      <c r="E18" s="5">
+      <c r="F18" s="5">
         <v>-3.9</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>27</v>
@@ -709,16 +821,19 @@
       <c r="C19" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="5">
-        <v>80.1</v>
+      <c r="D19" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="E19" s="5">
+        <v>80.099999999999994</v>
+      </c>
+      <c r="F19" s="5">
         <v>-38.6</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>29</v>
@@ -726,16 +841,19 @@
       <c r="C20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="5">
-        <v>76.4</v>
+      <c r="D20" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="E20" s="5">
-        <v>9.3</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="F20" s="5">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>31</v>
@@ -743,56 +861,59 @@
       <c r="C21" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="5">
         <v>64.7</v>
       </c>
-      <c r="E21" s="5">
-        <v>3.0</v>
+      <c r="F21" s="5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="C2"/>
-    <hyperlink r:id="rId3" ref="B3"/>
-    <hyperlink r:id="rId4" ref="C3"/>
-    <hyperlink r:id="rId5" ref="B4"/>
-    <hyperlink r:id="rId6" ref="C4"/>
-    <hyperlink r:id="rId7" ref="B5"/>
-    <hyperlink r:id="rId8" ref="C5"/>
-    <hyperlink r:id="rId9" ref="B6"/>
-    <hyperlink r:id="rId10" ref="C6"/>
-    <hyperlink r:id="rId11" ref="B7"/>
-    <hyperlink r:id="rId12" ref="C7"/>
-    <hyperlink r:id="rId13" ref="B8"/>
-    <hyperlink r:id="rId14" ref="C8"/>
-    <hyperlink r:id="rId15" ref="B9"/>
-    <hyperlink r:id="rId16" ref="C9"/>
-    <hyperlink r:id="rId17" ref="B10"/>
-    <hyperlink r:id="rId18" ref="C10"/>
-    <hyperlink r:id="rId19" ref="B11"/>
-    <hyperlink r:id="rId20" ref="C11"/>
-    <hyperlink r:id="rId21" ref="B12"/>
-    <hyperlink r:id="rId22" ref="C12"/>
-    <hyperlink r:id="rId23" ref="B13"/>
-    <hyperlink r:id="rId24" ref="C13"/>
-    <hyperlink r:id="rId25" ref="B14"/>
-    <hyperlink r:id="rId26" ref="C14"/>
-    <hyperlink r:id="rId27" ref="B15"/>
-    <hyperlink r:id="rId28" ref="C15"/>
-    <hyperlink r:id="rId29" ref="B16"/>
-    <hyperlink r:id="rId30" ref="C16"/>
-    <hyperlink r:id="rId31" ref="B17"/>
-    <hyperlink r:id="rId32" ref="C17"/>
-    <hyperlink r:id="rId33" ref="B18"/>
-    <hyperlink r:id="rId34" ref="C18"/>
-    <hyperlink r:id="rId35" ref="B19"/>
-    <hyperlink r:id="rId36" ref="C19"/>
-    <hyperlink r:id="rId37" ref="B20"/>
-    <hyperlink r:id="rId38" ref="C20"/>
-    <hyperlink r:id="rId39" ref="B21"/>
-    <hyperlink r:id="rId40" ref="C21"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="B4" r:id="rId5"/>
+    <hyperlink ref="C4" r:id="rId6"/>
+    <hyperlink ref="B5" r:id="rId7"/>
+    <hyperlink ref="C5" r:id="rId8"/>
+    <hyperlink ref="B6" r:id="rId9"/>
+    <hyperlink ref="C6" r:id="rId10"/>
+    <hyperlink ref="B7" r:id="rId11"/>
+    <hyperlink ref="C7" r:id="rId12"/>
+    <hyperlink ref="B8" r:id="rId13"/>
+    <hyperlink ref="C8" r:id="rId14"/>
+    <hyperlink ref="B9" r:id="rId15"/>
+    <hyperlink ref="C9" r:id="rId16"/>
+    <hyperlink ref="B10" r:id="rId17"/>
+    <hyperlink ref="C10" r:id="rId18"/>
+    <hyperlink ref="B11" r:id="rId19"/>
+    <hyperlink ref="C11" r:id="rId20"/>
+    <hyperlink ref="B12" r:id="rId21"/>
+    <hyperlink ref="C12" r:id="rId22"/>
+    <hyperlink ref="B13" r:id="rId23"/>
+    <hyperlink ref="C13" r:id="rId24"/>
+    <hyperlink ref="B14" r:id="rId25"/>
+    <hyperlink ref="C14" r:id="rId26"/>
+    <hyperlink ref="B15" r:id="rId27"/>
+    <hyperlink ref="C15" r:id="rId28"/>
+    <hyperlink ref="B16" r:id="rId29"/>
+    <hyperlink ref="C16" r:id="rId30"/>
+    <hyperlink ref="B17" r:id="rId31"/>
+    <hyperlink ref="C17" r:id="rId32"/>
+    <hyperlink ref="B18" r:id="rId33"/>
+    <hyperlink ref="C18" r:id="rId34"/>
+    <hyperlink ref="B19" r:id="rId35"/>
+    <hyperlink ref="C19" r:id="rId36"/>
+    <hyperlink ref="B20" r:id="rId37"/>
+    <hyperlink ref="C20" r:id="rId38"/>
+    <hyperlink ref="B21" r:id="rId39"/>
+    <hyperlink ref="C21" r:id="rId40"/>
   </hyperlinks>
-  <drawing r:id="rId41"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
filtro cartola uf xlxs
</commit_message>
<xml_diff>
--- a/clubes.xlsx
+++ b/clubes.xlsx
@@ -117,9 +117,6 @@
     <t>Ceará</t>
   </si>
   <si>
-    <t>UF</t>
-  </si>
-  <si>
     <t>SP</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
   </si>
   <si>
     <t>CE</t>
+  </si>
+  <si>
+    <t>uf</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -460,7 +460,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -482,7 +482,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="5">
         <v>688.6</v>
@@ -502,7 +502,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" s="5">
         <v>543</v>
@@ -522,7 +522,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="5">
         <v>466.9</v>
@@ -542,7 +542,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="5">
         <v>424.5</v>
@@ -562,7 +562,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="5">
         <v>402</v>
@@ -582,7 +582,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="5">
         <v>386.8</v>
@@ -602,7 +602,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="5">
         <v>297.3</v>
@@ -622,7 +622,7 @@
         <v>11</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" s="5">
         <v>293.2</v>
@@ -642,7 +642,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="5">
         <v>260.89999999999998</v>
@@ -662,7 +662,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="5">
         <v>257.89999999999998</v>
@@ -682,7 +682,7 @@
         <v>6</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="5">
         <v>217.7</v>
@@ -702,7 +702,7 @@
         <v>20</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" s="5">
         <v>207.4</v>
@@ -722,7 +722,7 @@
         <v>8</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14" s="5">
         <v>182.9</v>
@@ -742,7 +742,7 @@
         <v>22</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" s="5">
         <v>136.1</v>
@@ -762,7 +762,7 @@
         <v>24</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E16" s="5">
         <v>104.1</v>
@@ -782,7 +782,7 @@
         <v>20</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E17" s="5">
         <v>102.8</v>
@@ -802,7 +802,7 @@
         <v>22</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E18" s="5">
         <v>88.3</v>
@@ -822,7 +822,7 @@
         <v>28</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E19" s="5">
         <v>80.099999999999994</v>
@@ -842,7 +842,7 @@
         <v>30</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E20" s="5">
         <v>76.400000000000006</v>
@@ -862,7 +862,7 @@
         <v>31</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" s="5">
         <v>64.7</v>

</xml_diff>